<commit_message>
revisi format laporan pembelian dan laporan penjualan
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/Format Laporan/3. format laporan pembelian.xlsx
+++ b/Documen Aturusaha/Format Laporan/3. format laporan pembelian.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="15255" windowHeight="7905" tabRatio="786" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="15255" windowHeight="7905" tabRatio="699" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Pesanan Pembelian" sheetId="14" r:id="rId1"/>
     <sheet name="Pembelian" sheetId="19" r:id="rId2"/>
     <sheet name="pengecekkan brg" sheetId="16" r:id="rId3"/>
+    <sheet name="return pembelian" sheetId="20" r:id="rId4"/>
+    <sheet name="hutang" sheetId="21" r:id="rId5"/>
+    <sheet name="pembayaran" sheetId="22" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="108">
   <si>
     <t>NO</t>
   </si>
@@ -30,18 +33,6 @@
     <t>Halaman Preview</t>
   </si>
   <si>
-    <t>Keterangan</t>
-  </si>
-  <si>
-    <t>p_barang.speca_brg</t>
-  </si>
-  <si>
-    <t>p_barang.merk_brg</t>
-  </si>
-  <si>
-    <t>p_barangsatuan_brg</t>
-  </si>
-  <si>
     <t>Tgl Transaksi</t>
   </si>
   <si>
@@ -51,27 +42,9 @@
     <t>tgl akhir</t>
   </si>
   <si>
-    <t>Stok Fisik</t>
-  </si>
-  <si>
-    <t>Selisih</t>
-  </si>
-  <si>
     <t>Petugas</t>
   </si>
   <si>
-    <t>p_stok_opname.stok_akhir</t>
-  </si>
-  <si>
-    <t>p_stok_opname.bukti_fisik</t>
-  </si>
-  <si>
-    <t>p_stok_opname.selisih</t>
-  </si>
-  <si>
-    <t>p_stok_opname.petugas</t>
-  </si>
-  <si>
     <t>Print</t>
   </si>
   <si>
@@ -123,9 +96,6 @@
     <t>p_po.id_supplier</t>
   </si>
   <si>
-    <t>sum(p_detail_po.jumlah_harga)</t>
-  </si>
-  <si>
     <t>p_po.diskon_tambahan</t>
   </si>
   <si>
@@ -168,30 +138,15 @@
     <t>p_order.metode_bayar</t>
   </si>
   <si>
-    <t>sum(p_detail_order.jumlah_harga)</t>
-  </si>
-  <si>
     <t>Laporan pengecekkan brg</t>
   </si>
   <si>
     <t>Tgl pengecekkan</t>
   </si>
   <si>
-    <t>p_cek_barang.creat_at</t>
-  </si>
-  <si>
     <t>No Order</t>
   </si>
   <si>
-    <t>p_cek_barang.id_order</t>
-  </si>
-  <si>
-    <t>Sesuai</t>
-  </si>
-  <si>
-    <t>Tidak sesuai</t>
-  </si>
-  <si>
     <t>Kondisi Barang</t>
   </si>
   <si>
@@ -199,13 +154,202 @@
   </si>
   <si>
     <t>Cacat</t>
+  </si>
+  <si>
+    <t>Diterima</t>
+  </si>
+  <si>
+    <t>Kurang</t>
+  </si>
+  <si>
+    <t>Tgl Diterima</t>
+  </si>
+  <si>
+    <t>p_order.tgl_tiba where p_cek_barang.id_order</t>
+  </si>
+  <si>
+    <t>p_order.no_order where p_cek_barang.id_order</t>
+  </si>
+  <si>
+    <t>sum(p_detail_cek.jum_sesuai)</t>
+  </si>
+  <si>
+    <t>sum(p_detail_cek.jum_no_sesuai)</t>
+  </si>
+  <si>
+    <t>sum(p_detail_cek.kualitas_sesuai)</t>
+  </si>
+  <si>
+    <t>sum(p_detail_cek.kualitas_no_sesuai)</t>
+  </si>
+  <si>
+    <t>p_cek_brg_id_karyawan</t>
+  </si>
+  <si>
+    <t>Tgl complain</t>
+  </si>
+  <si>
+    <t>p_cek_brg.tgl_konfirm_cek</t>
+  </si>
+  <si>
+    <t>Respon Supplier</t>
+  </si>
+  <si>
+    <t>Tgl Respon</t>
+  </si>
+  <si>
+    <t>Ditolak</t>
+  </si>
+  <si>
+    <t>p_cek_brg.tgl_respon_supplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(sum(p_detail_cek.jum_no_sesuai) where p_detail_cek.status_return = 1)  + (sum(p_detail_kualitas_no_sesuai) where p_detail_cek.status_return = 1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(sum(p_detail_cek.jum_no_sesuai) where p_detail_cek.status_return = 0)  + (sum(p_detail_kualitas_no_sesuai) where p_detail_cek.status_return = 0) </t>
+  </si>
+  <si>
+    <t>p_cek_barang.creat_at beetween tgl_awal and tgl akhir yg di input user</t>
+  </si>
+  <si>
+    <t>Tgl Return</t>
+  </si>
+  <si>
+    <t>p_order.tgl_tiba where p_return_pembelian.id_order</t>
+  </si>
+  <si>
+    <t>p_return_pembelian.tgl_return</t>
+  </si>
+  <si>
+    <t>Jenis Return</t>
+  </si>
+  <si>
+    <t>p_return_pembelian.jenis_return</t>
+  </si>
+  <si>
+    <t>Laporan Return Pembelian</t>
+  </si>
+  <si>
+    <t>Ongkir Return</t>
+  </si>
+  <si>
+    <t>p_return_pembelian.ongkir_return</t>
+  </si>
+  <si>
+    <t>print</t>
+  </si>
+  <si>
+    <t>p_order.id_suplier where p_order.id = p_return_pembelian.id_order</t>
+  </si>
+  <si>
+    <t>supplier</t>
+  </si>
+  <si>
+    <t>defaul all supplier</t>
+  </si>
+  <si>
+    <t>Laporan Hutang</t>
+  </si>
+  <si>
+    <t>p_order.id_suplier</t>
+  </si>
+  <si>
+    <t>Tgl Order</t>
+  </si>
+  <si>
+    <t>Jumlah hutang</t>
+  </si>
+  <si>
+    <t>p_order.kurang_bayar</t>
+  </si>
+  <si>
+    <t>Status pembayaran</t>
+  </si>
+  <si>
+    <t>p_order.status_bayar</t>
+  </si>
+  <si>
+    <t>Tgl jatuh tempo</t>
+  </si>
+  <si>
+    <t>p_oreer.tgl_jatuh_tempo</t>
+  </si>
+  <si>
+    <t>status Bayar</t>
+  </si>
+  <si>
+    <t>lunas</t>
+  </si>
+  <si>
+    <t>belum lunas</t>
+  </si>
+  <si>
+    <t>Tgl bayar</t>
+  </si>
+  <si>
+    <t>Jumlah bayar</t>
+  </si>
+  <si>
+    <t>bank tujuan</t>
+  </si>
+  <si>
+    <t>metode bayar</t>
+  </si>
+  <si>
+    <t>Laporan pembayaran</t>
+  </si>
+  <si>
+    <t>Tunai</t>
+  </si>
+  <si>
+    <t>status Pembelian</t>
+  </si>
+  <si>
+    <t>Kredit</t>
+  </si>
+  <si>
+    <t>p_bayar.tgl_bayar</t>
+  </si>
+  <si>
+    <t>p_bayar.jumlah_bayar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bank asal </t>
+  </si>
+  <si>
+    <t>p_bayar.bank_asal (nm bank, no rek, atas nama)</t>
+  </si>
+  <si>
+    <t>p_bayar.bank_tujuan (nm bank, no rek, atas nama)</t>
+  </si>
+  <si>
+    <t>p_bayar.metode_bayar</t>
+  </si>
+  <si>
+    <t>p_bayar where   tgl_bayar between tgl awal and tgl akhir and mont(tgl bayar) = bulan ini</t>
+  </si>
+  <si>
+    <t>p_po.total</t>
+  </si>
+  <si>
+    <t>p_order.total</t>
+  </si>
+  <si>
+    <t>wajib di pilih</t>
+  </si>
+  <si>
+    <t>boleh kosong</t>
+  </si>
+  <si>
+    <t>p_order where metode_bayar =1 and tgl_order between tgl awal and tgl akhir</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,16 +390,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,12 +418,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -299,7 +429,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -372,18 +502,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -415,9 +589,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -430,34 +601,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -473,6 +617,47 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -484,6 +669,45 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -782,7 +1006,7 @@
   <dimension ref="A2:I14"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:G4"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -799,15 +1023,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="13"/>
@@ -822,33 +1046,33 @@
     <row r="4" spans="1:9" s="2" customFormat="1">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
-      <c r="C4" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="39"/>
+      <c r="C4" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="29"/>
       <c r="G4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="26.25">
-      <c r="C5" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>23</v>
+      <c r="H4" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="C5" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="C6" s="4"/>
-      <c r="D6" s="37" t="s">
-        <v>24</v>
+      <c r="D6" s="27" t="s">
+        <v>14</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="4"/>
@@ -870,33 +1094,33 @@
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
+      <c r="A11" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
     </row>
@@ -905,55 +1129,55 @@
         <v>0</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>30</v>
-      </c>
       <c r="G12" s="10" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="38.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30">
       <c r="A13" s="14"/>
       <c r="B13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="I13" s="24" t="s">
         <v>27</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I13" s="34" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -982,7 +1206,7 @@
   <dimension ref="A2:K13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1000,54 +1224,54 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
-      <c r="C3" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="39"/>
+      <c r="C3" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="29"/>
       <c r="G3" s="4"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:11" ht="26.25">
-      <c r="C4" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="35"/>
+      <c r="C4" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="25"/>
       <c r="H4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="32" t="s">
-        <v>18</v>
+      <c r="J4" s="22" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="C5" s="4"/>
-      <c r="D5" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="33"/>
+      <c r="D5" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="23"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="4"/>
@@ -1073,39 +1297,39 @@
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
+      <c r="A10" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
     </row>
@@ -1114,67 +1338,67 @@
         <v>0</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>30</v>
-      </c>
       <c r="I11" s="10" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="38.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="30">
       <c r="A12" s="14"/>
       <c r="B12" s="15" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K12" s="34" t="s">
-        <v>49</v>
+        <v>26</v>
+      </c>
+      <c r="K12" s="24" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1202,36 +1426,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:K21"/>
+  <dimension ref="A2:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:13">
+      <c r="A2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-    </row>
-    <row r="3" spans="1:11" s="2" customFormat="1">
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -1239,225 +1469,886 @@
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="C4" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="22"/>
-      <c r="H4" s="6" t="s">
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="D4" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="F4" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="21"/>
+      <c r="I4" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
-      <c r="C5" s="4"/>
+    <row r="5" spans="1:13">
       <c r="D5" s="4"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="C6" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:13">
       <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="4"/>
+      <c r="F7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="2" customFormat="1">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="29" t="s">
+    <row r="8" spans="1:13" s="2" customFormat="1">
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="41"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="51"/>
+    </row>
+    <row r="11" spans="1:13" s="9" customFormat="1">
+      <c r="A11" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="46"/>
+      <c r="G11" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="48"/>
+      <c r="I11" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="K11" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="L11" s="56"/>
+      <c r="M11" s="48"/>
+    </row>
+    <row r="12" spans="1:13" s="9" customFormat="1">
+      <c r="A12" s="53"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="55"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="153">
+      <c r="A13" s="14"/>
+      <c r="B13" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="31"/>
-    </row>
-    <row r="11" spans="1:11" s="9" customFormat="1">
-      <c r="A11" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="12" t="s">
+      <c r="G13" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="H13" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="43"/>
-      <c r="H11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="9" customFormat="1">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="12" t="s">
+      <c r="J13" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="10" t="s">
+      <c r="K13" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-    </row>
-    <row r="13" spans="1:11" ht="38.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="L13" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="M13" s="34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
-      <c r="E14" s="17"/>
+      <c r="E14" s="16"/>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="H14" s="17"/>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
-      <c r="C15" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="C15" s="16"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+    </row>
+    <row r="16" spans="1:13" s="3" customFormat="1" ht="37.5" customHeight="1">
+      <c r="D16" s="11"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="44"/>
+    </row>
+    <row r="17" spans="4:11" s="3" customFormat="1">
+      <c r="D17" s="11"/>
+      <c r="E17" s="19"/>
+    </row>
+    <row r="18" spans="4:11">
+      <c r="H18" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11">
+      <c r="F20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="E15:L15"/>
+    <mergeCell ref="E16:L16"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="I11:I12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:H19"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="6" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8">
+      <c r="A2" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+    </row>
+    <row r="3" spans="1:8" s="2" customFormat="1">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="C4" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="F4" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="C6" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="C8" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="F9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1">
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="H10"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="41"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+    </row>
+    <row r="13" spans="1:8" s="9" customFormat="1">
+      <c r="A13" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="54" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="9" customFormat="1">
+      <c r="A14" s="53"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+    </row>
+    <row r="15" spans="1:8" ht="63.75">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-    </row>
-    <row r="17" spans="3:11" s="3" customFormat="1" ht="37.5" customHeight="1">
-      <c r="C17" s="11"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-    </row>
-    <row r="18" spans="3:11" s="3" customFormat="1">
-      <c r="C18" s="11"/>
-      <c r="D18" s="20"/>
-    </row>
-    <row r="19" spans="3:11">
-      <c r="G19" t="s">
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="31"/>
+    </row>
+    <row r="18" spans="1:6" s="3" customFormat="1" ht="37.5" customHeight="1">
+      <c r="E18" s="30"/>
+      <c r="F18" s="32"/>
+    </row>
+    <row r="19" spans="1:6" s="3" customFormat="1">
+      <c r="E19" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:I21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9">
+      <c r="A2" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+    </row>
+    <row r="3" spans="1:9" s="2" customFormat="1">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="D4" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="G5" s="35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="D6" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="J19" t="s">
+    </row>
+    <row r="8" spans="1:9">
+      <c r="D8" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="D10" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="E11" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="2" customFormat="1">
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="I12"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+    </row>
+    <row r="15" spans="1:9" s="9" customFormat="1">
+      <c r="A15" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="G15" s="54" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="9" customFormat="1">
+      <c r="A16" s="53"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="55"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="1:7" s="3" customFormat="1" ht="37.5" customHeight="1">
+      <c r="G20" s="30"/>
+    </row>
+    <row r="21" spans="1:7" s="3" customFormat="1">
+      <c r="D21" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="3:11">
-      <c r="E21" t="s">
+      <c r="G21" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="G15:G16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:I21"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9">
+      <c r="A2" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+    </row>
+    <row r="3" spans="1:9" s="2" customFormat="1">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="D4" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="G5" s="35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="D6" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:9">
+      <c r="D8" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="D10" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="E11" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="2" customFormat="1">
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="I12"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="51"/>
+    </row>
+    <row r="15" spans="1:9" s="9" customFormat="1">
+      <c r="A15" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="G15" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" s="58" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="9" customFormat="1">
+      <c r="A16" s="53"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="59"/>
+    </row>
+    <row r="17" spans="1:8" ht="38.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="1:8" s="3" customFormat="1" ht="37.5" customHeight="1">
+      <c r="G20" s="30"/>
+    </row>
+    <row r="21" spans="1:8" s="3" customFormat="1">
+      <c r="G21" s="30"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="H15:H16"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="A10:J10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="G15:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>